<commit_message>
serie democracia grafico y texto
</commit_message>
<xml_diff>
--- a/data/latino/demo_serie.xlsx
+++ b/data/latino/demo_serie.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Dropbox\Trabajo\UMAD\Piso I\Piso-I-OP\data\latino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00E2CFE3-B229-402B-85C8-16DCE035E1AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD20AF7-270C-49A1-BBD5-15E831A72384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AD358659-11C2-4884-80AD-7F71002222F1}"/>
   </bookViews>
@@ -613,8 +613,8 @@
   <dimension ref="A1:AG143"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F140" sqref="F140"/>
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C46" sqref="C46:C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -645,7 +645,7 @@
         <v>0.85599999999999998</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
         <v>29</v>
@@ -659,7 +659,7 @@
         <v>0.82599999999999996</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
         <v>29</v>
@@ -673,7 +673,7 @@
         <v>0.87599999999999989</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
         <v>29</v>
@@ -687,7 +687,7 @@
         <v>0.83200000000000007</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
         <v>29</v>
@@ -701,7 +701,7 @@
         <v>0.84299999999999997</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s">
         <v>29</v>
@@ -739,7 +739,7 @@
         <v>0.81599999999999995</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s">
         <v>29</v>
@@ -777,7 +777,7 @@
         <v>0.79599999999999993</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
         <v>29</v>
@@ -815,7 +815,7 @@
         <v>0.79900000000000004</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
         <v>29</v>
@@ -853,7 +853,7 @@
         <v>0.82299999999999995</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D10" t="s">
         <v>29</v>
@@ -867,7 +867,7 @@
         <v>0.81799999999999995</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D11" t="s">
         <v>29</v>
@@ -881,7 +881,7 @@
         <v>0.80500000000000005</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D12" t="s">
         <v>29</v>
@@ -895,7 +895,7 @@
         <v>0.78099999999999992</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D13" t="s">
         <v>29</v>
@@ -909,7 +909,7 @@
         <v>0.81900000000000006</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D14" t="s">
         <v>29</v>
@@ -923,7 +923,7 @@
         <v>0.84900000000000009</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D15" t="s">
         <v>29</v>
@@ -937,7 +937,7 @@
         <v>0.78</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D16" t="s">
         <v>29</v>
@@ -951,7 +951,7 @@
         <v>0.78799999999999992</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D17" t="s">
         <v>29</v>
@@ -965,7 +965,7 @@
         <v>0.748</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D18" t="s">
         <v>29</v>
@@ -979,7 +979,7 @@
         <v>0.77700000000000002</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D19" t="s">
         <v>29</v>
@@ -993,7 +993,7 @@
         <v>0.71299999999999997</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D20" t="s">
         <v>29</v>
@@ -1007,7 +1007,7 @@
         <v>0.72900000000000009</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D21" t="s">
         <v>29</v>
@@ -1021,7 +1021,7 @@
         <v>0.64500000000000002</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D22" t="s">
         <v>29</v>
@@ -1035,7 +1035,7 @@
         <v>0.78500000000000003</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D23" t="s">
         <v>29</v>
@@ -1357,7 +1357,7 @@
         <v>6.2E-2</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D46" t="s">
         <v>29</v>
@@ -1371,7 +1371,7 @@
         <v>7.9000000000000001E-2</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D47" t="s">
         <v>29</v>
@@ -1385,7 +1385,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D48" t="s">
         <v>29</v>
@@ -1399,7 +1399,7 @@
         <v>7.0999999999999994E-2</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D49" t="s">
         <v>29</v>
@@ -1413,7 +1413,7 @@
         <v>6.2E-2</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D50" t="s">
         <v>29</v>
@@ -1427,7 +1427,7 @@
         <v>8.199999999999999E-2</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D51" t="s">
         <v>29</v>
@@ -1441,7 +1441,7 @@
         <v>9.5000000000000001E-2</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D52" t="s">
         <v>29</v>
@@ -1455,7 +1455,7 @@
         <v>0.109</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D53" t="s">
         <v>29</v>
@@ -1469,7 +1469,7 @@
         <v>0.105</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D54" t="s">
         <v>29</v>
@@ -1483,7 +1483,7 @@
         <v>7.8E-2</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D55" t="s">
         <v>29</v>
@@ -1497,7 +1497,7 @@
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D56" t="s">
         <v>29</v>
@@ -1511,7 +1511,7 @@
         <v>0.114</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D57" t="s">
         <v>29</v>
@@ -1525,7 +1525,7 @@
         <v>0.11800000000000001</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D58" t="s">
         <v>29</v>
@@ -1539,7 +1539,7 @@
         <v>6.9000000000000006E-2</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D59" t="s">
         <v>29</v>
@@ -1553,7 +1553,7 @@
         <v>6.2E-2</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D60" t="s">
         <v>29</v>
@@ -1567,7 +1567,7 @@
         <v>9.1999999999999998E-2</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D61" t="s">
         <v>29</v>
@@ -1581,7 +1581,7 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D62" t="s">
         <v>29</v>
@@ -1595,7 +1595,7 @@
         <v>0.114</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D63" t="s">
         <v>29</v>
@@ -1609,7 +1609,7 @@
         <v>0.16500000000000001</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D64" t="s">
         <v>29</v>
@@ -1623,7 +1623,7 @@
         <v>0.13200000000000001</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D65" t="s">
         <v>29</v>
@@ -1637,7 +1637,7 @@
         <v>0.19</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D66" t="s">
         <v>29</v>
@@ -1651,7 +1651,7 @@
         <v>0.13300000000000001</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D67" t="s">
         <v>29</v>

</xml_diff>